<commit_message>
year was 2017 changed to 2016
</commit_message>
<xml_diff>
--- a/Data/Ballard Locks Fish Counts/BallardLocksFinal2016 - daily.xlsx
+++ b/Data/Ballard Locks Fish Counts/BallardLocksFinal2016 - daily.xlsx
@@ -1,16 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elizabeth Allyn\Documents\GitHub\PinnipedCaseStudies\Data\Ballard Locks Fish Counts\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5847B47-DE9A-4F2A-8CAF-BEEE277D1C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="108" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="1125" yWindow="660" windowWidth="24960" windowHeight="14355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Counts" sheetId="1" r:id="rId1"/>
     <sheet name="Historical" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -116,7 +133,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
@@ -366,11 +383,11 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -378,7 +395,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -399,12 +416,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1146,6 +1166,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5B0F-4C3C-9ED2-34F3BB68D435}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1868,6 +1893,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5B0F-4C3C-9ED2-34F3BB68D435}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1961,7 +1991,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1990,7 +2019,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2732,6 +2761,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-083E-4194-963C-28B196C070C9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3454,6 +3488,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-083E-4194-963C-28B196C070C9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3547,7 +3586,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3576,7 +3614,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3832,6 +3870,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F26B-4738-BF03-07166BC1D1A4}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -4068,6 +4111,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F26B-4738-BF03-07166BC1D1A4}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4161,7 +4209,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4190,7 +4237,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4932,6 +4979,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0D0E-497C-BFA7-C25AC1FD10DB}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -5654,6 +5706,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0D0E-497C-BFA7-C25AC1FD10DB}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -5747,7 +5804,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5776,7 +5832,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6518,6 +6574,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B6FC-49F0-BD07-C6933782A2D9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -7240,6 +7301,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B6FC-49F0-BD07-C6933782A2D9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -7333,7 +7399,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7362,7 +7427,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -7618,6 +7683,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F043-4FC5-A76A-032DDAEC7EC9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -7854,6 +7924,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F043-4FC5-A76A-032DDAEC7EC9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -7947,7 +8022,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7992,7 +8066,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8022,7 +8102,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8054,7 +8140,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8086,7 +8178,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8118,7 +8216,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8150,7 +8254,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8171,9 +8281,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -8211,7 +8321,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -8283,7 +8393,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8456,43 +8566,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1188" topLeftCell="A79" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1185" activePane="bottomLeft"/>
       <selection activeCell="AL1" sqref="AL1:AL1048576"/>
-      <selection pane="bottomLeft" activeCell="K119" sqref="K119"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:A116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="6.77734375" style="2" customWidth="1"/>
-    <col min="6" max="7" width="8.33203125" style="2" customWidth="1"/>
-    <col min="8" max="10" width="6.77734375" style="2" customWidth="1"/>
-    <col min="11" max="12" width="4.77734375" style="6" customWidth="1"/>
-    <col min="13" max="13" width="6.77734375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="4.77734375" style="6" customWidth="1"/>
-    <col min="15" max="16" width="6.77734375" style="2" customWidth="1"/>
-    <col min="17" max="18" width="4.77734375" style="6" customWidth="1"/>
-    <col min="19" max="20" width="8.33203125" style="2" customWidth="1"/>
-    <col min="21" max="23" width="6.77734375" style="2" customWidth="1"/>
-    <col min="24" max="25" width="4.77734375" style="6" customWidth="1"/>
-    <col min="26" max="26" width="6.77734375" style="2" customWidth="1"/>
-    <col min="27" max="27" width="4.77734375" style="6" customWidth="1"/>
-    <col min="28" max="29" width="6.77734375" style="2" customWidth="1"/>
-    <col min="30" max="31" width="4.77734375" style="6" customWidth="1"/>
-    <col min="32" max="32" width="6.77734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="6.7109375" style="2" customWidth="1"/>
+    <col min="6" max="7" width="8.28515625" style="2" customWidth="1"/>
+    <col min="8" max="10" width="6.7109375" style="2" customWidth="1"/>
+    <col min="11" max="12" width="4.7109375" style="6" customWidth="1"/>
+    <col min="13" max="13" width="6.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="4.7109375" style="6" customWidth="1"/>
+    <col min="15" max="16" width="6.7109375" style="2" customWidth="1"/>
+    <col min="17" max="18" width="4.7109375" style="6" customWidth="1"/>
+    <col min="19" max="20" width="8.28515625" style="2" customWidth="1"/>
+    <col min="21" max="23" width="6.7109375" style="2" customWidth="1"/>
+    <col min="24" max="25" width="4.7109375" style="6" customWidth="1"/>
+    <col min="26" max="26" width="6.7109375" style="2" customWidth="1"/>
+    <col min="27" max="27" width="4.7109375" style="6" customWidth="1"/>
+    <col min="28" max="29" width="6.7109375" style="2" customWidth="1"/>
+    <col min="30" max="31" width="4.7109375" style="6" customWidth="1"/>
+    <col min="32" max="32" width="6.7109375" style="2" customWidth="1"/>
     <col min="33" max="33" width="11" style="2" customWidth="1"/>
-    <col min="34" max="34" width="6.77734375" style="2" customWidth="1"/>
+    <col min="34" max="34" width="6.7109375" style="2" customWidth="1"/>
     <col min="35" max="35" width="11" style="2" customWidth="1"/>
-    <col min="36" max="36" width="6.77734375" style="2" customWidth="1"/>
+    <col min="36" max="36" width="6.7109375" style="2" customWidth="1"/>
     <col min="37" max="37" width="11" style="2" customWidth="1"/>
-    <col min="38" max="16384" width="8.88671875" style="2"/>
+    <col min="38" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
@@ -8506,7 +8616,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -8564,7 +8674,7 @@
       </c>
       <c r="AK2" s="27"/>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -8680,9 +8790,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>42898</v>
+        <v>42533</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -8804,9 +8914,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>42899</v>
+        <v>42534</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
@@ -8928,9 +9038,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>42900</v>
+        <v>42535</v>
       </c>
       <c r="B6" s="2">
         <v>4</v>
@@ -9052,9 +9162,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>42901</v>
+        <v>42536</v>
       </c>
       <c r="B7" s="2">
         <v>5</v>
@@ -9176,9 +9286,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>42902</v>
+        <v>42537</v>
       </c>
       <c r="B8" s="2">
         <v>5</v>
@@ -9300,9 +9410,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>42903</v>
+        <v>42538</v>
       </c>
       <c r="B9" s="2">
         <v>2</v>
@@ -9424,9 +9534,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>42904</v>
+        <v>42539</v>
       </c>
       <c r="B10" s="2">
         <v>2</v>
@@ -9548,9 +9658,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>42905</v>
+        <v>42540</v>
       </c>
       <c r="B11" s="2">
         <v>4</v>
@@ -9672,9 +9782,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>42906</v>
+        <v>42541</v>
       </c>
       <c r="B12" s="2">
         <v>4</v>
@@ -9796,9 +9906,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>42907</v>
+        <v>42542</v>
       </c>
       <c r="B13" s="2">
         <v>3</v>
@@ -9920,9 +10030,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>42908</v>
+        <v>42543</v>
       </c>
       <c r="B14" s="2">
         <v>2</v>
@@ -10044,9 +10154,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>42909</v>
+        <v>42544</v>
       </c>
       <c r="B15" s="2">
         <v>2</v>
@@ -10168,9 +10278,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>42910</v>
+        <v>42545</v>
       </c>
       <c r="B16" s="2">
         <v>3</v>
@@ -10292,9 +10402,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>42911</v>
+        <v>42546</v>
       </c>
       <c r="B17" s="2">
         <v>0</v>
@@ -10416,9 +10526,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>42912</v>
+        <v>42547</v>
       </c>
       <c r="B18" s="2">
         <v>5</v>
@@ -10540,9 +10650,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>42913</v>
+        <v>42548</v>
       </c>
       <c r="B19" s="2">
         <v>1</v>
@@ -10664,9 +10774,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>42914</v>
+        <v>42549</v>
       </c>
       <c r="B20" s="2">
         <v>3</v>
@@ -10788,9 +10898,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>42915</v>
+        <v>42550</v>
       </c>
       <c r="B21" s="2">
         <v>2</v>
@@ -10912,9 +11022,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>42916</v>
+        <v>42551</v>
       </c>
       <c r="B22" s="2">
         <v>5</v>
@@ -11036,9 +11146,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>42917</v>
+        <v>42552</v>
       </c>
       <c r="B23" s="2">
         <v>4</v>
@@ -11160,9 +11270,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>42918</v>
+        <v>42553</v>
       </c>
       <c r="B24" s="2">
         <v>3</v>
@@ -11284,9 +11394,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>42919</v>
+        <v>42554</v>
       </c>
       <c r="B25" s="2">
         <v>2</v>
@@ -11408,9 +11518,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>42920</v>
+        <v>42555</v>
       </c>
       <c r="B26" s="2">
         <v>5</v>
@@ -11532,9 +11642,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
-        <v>42921</v>
+        <v>42556</v>
       </c>
       <c r="B27" s="2">
         <v>2</v>
@@ -11656,9 +11766,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
-        <v>42922</v>
+        <v>42557</v>
       </c>
       <c r="B28" s="2">
         <v>4</v>
@@ -11780,9 +11890,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>42923</v>
+        <v>42558</v>
       </c>
       <c r="B29" s="2">
         <v>1</v>
@@ -11904,9 +12014,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
-        <v>42924</v>
+        <v>42559</v>
       </c>
       <c r="B30" s="2">
         <v>0</v>
@@ -12028,9 +12138,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
-        <v>42925</v>
+        <v>42560</v>
       </c>
       <c r="B31" s="2">
         <v>1</v>
@@ -12152,9 +12262,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
-        <v>42926</v>
+        <v>42561</v>
       </c>
       <c r="B32" s="2">
         <v>2</v>
@@ -12276,9 +12386,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
-        <v>42927</v>
+        <v>42562</v>
       </c>
       <c r="B33" s="2">
         <v>2</v>
@@ -12400,9 +12510,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
-        <v>42928</v>
+        <v>42563</v>
       </c>
       <c r="B34" s="2">
         <v>2</v>
@@ -12524,9 +12634,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
-        <v>42929</v>
+        <v>42564</v>
       </c>
       <c r="B35" s="2">
         <v>5</v>
@@ -12648,9 +12758,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
-        <v>42930</v>
+        <v>42565</v>
       </c>
       <c r="B36" s="2">
         <v>0</v>
@@ -12772,9 +12882,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
-        <v>42931</v>
+        <v>42566</v>
       </c>
       <c r="B37" s="2">
         <v>2</v>
@@ -12896,9 +13006,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
-        <v>42932</v>
+        <v>42567</v>
       </c>
       <c r="B38" s="2">
         <v>2</v>
@@ -13020,9 +13130,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
-        <v>42933</v>
+        <v>42568</v>
       </c>
       <c r="B39" s="2">
         <v>4</v>
@@ -13144,9 +13254,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
-        <v>42934</v>
+        <v>42569</v>
       </c>
       <c r="B40" s="2">
         <v>2</v>
@@ -13268,9 +13378,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
-        <v>42935</v>
+        <v>42570</v>
       </c>
       <c r="B41" s="2">
         <v>2</v>
@@ -13392,9 +13502,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
-        <v>42936</v>
+        <v>42571</v>
       </c>
       <c r="B42" s="2">
         <v>2</v>
@@ -13516,9 +13626,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
-        <v>42937</v>
+        <v>42572</v>
       </c>
       <c r="B43" s="2">
         <v>0</v>
@@ -13640,9 +13750,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
-        <v>42938</v>
+        <v>42573</v>
       </c>
       <c r="B44" s="2">
         <v>3</v>
@@ -13764,9 +13874,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
-        <v>42939</v>
+        <v>42574</v>
       </c>
       <c r="B45" s="2">
         <v>3</v>
@@ -13888,9 +13998,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
-        <v>42940</v>
+        <v>42575</v>
       </c>
       <c r="B46" s="2">
         <v>3</v>
@@ -14012,9 +14122,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
-        <v>42941</v>
+        <v>42576</v>
       </c>
       <c r="B47" s="2">
         <v>3</v>
@@ -14136,9 +14246,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
-        <v>42942</v>
+        <v>42577</v>
       </c>
       <c r="B48" s="2">
         <v>2</v>
@@ -14260,9 +14370,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
-        <v>42943</v>
+        <v>42578</v>
       </c>
       <c r="B49" s="2">
         <v>3</v>
@@ -14384,9 +14494,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
-        <v>42944</v>
+        <v>42579</v>
       </c>
       <c r="B50" s="2">
         <v>3</v>
@@ -14508,9 +14618,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
-        <v>42945</v>
+        <v>42580</v>
       </c>
       <c r="B51" s="2">
         <v>2</v>
@@ -14632,9 +14742,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
-        <v>42946</v>
+        <v>42581</v>
       </c>
       <c r="B52" s="2">
         <v>3</v>
@@ -14756,9 +14866,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
-        <v>42947</v>
+        <v>42582</v>
       </c>
       <c r="B53" s="2">
         <v>5</v>
@@ -14880,9 +14990,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
-        <v>42948</v>
+        <v>42583</v>
       </c>
       <c r="B54" s="2">
         <v>4</v>
@@ -15008,9 +15118,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
-        <v>42949</v>
+        <v>42584</v>
       </c>
       <c r="B55" s="2">
         <v>6</v>
@@ -15136,9 +15246,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
-        <v>42950</v>
+        <v>42585</v>
       </c>
       <c r="B56" s="2">
         <v>2</v>
@@ -15264,9 +15374,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
-        <v>42951</v>
+        <v>42586</v>
       </c>
       <c r="B57" s="2">
         <v>4</v>
@@ -15392,9 +15502,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
-        <v>42952</v>
+        <v>42587</v>
       </c>
       <c r="B58" s="2">
         <v>4</v>
@@ -15520,9 +15630,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
-        <v>42953</v>
+        <v>42588</v>
       </c>
       <c r="B59" s="2">
         <v>3</v>
@@ -15648,9 +15758,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
-        <v>42954</v>
+        <v>42589</v>
       </c>
       <c r="B60" s="2">
         <v>3</v>
@@ -15776,9 +15886,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
-        <v>42955</v>
+        <v>42590</v>
       </c>
       <c r="B61" s="2">
         <v>1</v>
@@ -15904,9 +16014,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
-        <v>42956</v>
+        <v>42591</v>
       </c>
       <c r="B62" s="2">
         <v>2</v>
@@ -16032,9 +16142,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
-        <v>42957</v>
+        <v>42592</v>
       </c>
       <c r="B63" s="2">
         <v>2</v>
@@ -16160,9 +16270,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
-        <v>42958</v>
+        <v>42593</v>
       </c>
       <c r="B64" s="2">
         <v>4</v>
@@ -16288,9 +16398,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
-        <v>42959</v>
+        <v>42594</v>
       </c>
       <c r="B65" s="2">
         <v>2</v>
@@ -16416,9 +16526,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
-        <v>42960</v>
+        <v>42595</v>
       </c>
       <c r="B66" s="2">
         <v>3</v>
@@ -16544,9 +16654,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
-        <v>42961</v>
+        <v>42596</v>
       </c>
       <c r="B67" s="2">
         <v>4</v>
@@ -16672,9 +16782,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
-        <v>42962</v>
+        <v>42597</v>
       </c>
       <c r="B68" s="2">
         <v>3</v>
@@ -16800,9 +16910,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
-        <v>42963</v>
+        <v>42598</v>
       </c>
       <c r="B69" s="2">
         <v>3</v>
@@ -16928,9 +17038,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
-        <v>42964</v>
+        <v>42599</v>
       </c>
       <c r="B70" s="2">
         <v>7</v>
@@ -17056,9 +17166,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
-        <v>42965</v>
+        <v>42600</v>
       </c>
       <c r="B71" s="2">
         <v>4</v>
@@ -17184,9 +17294,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
-        <v>42966</v>
+        <v>42601</v>
       </c>
       <c r="B72" s="2">
         <v>3</v>
@@ -17312,9 +17422,9 @@
         <v>14.545454545454545</v>
       </c>
     </row>
-    <row r="73" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
-        <v>42967</v>
+        <v>42602</v>
       </c>
       <c r="B73" s="2">
         <v>3</v>
@@ -17440,9 +17550,9 @@
         <v>21.09090909090909</v>
       </c>
     </row>
-    <row r="74" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
-        <v>42968</v>
+        <v>42603</v>
       </c>
       <c r="B74" s="2">
         <v>4</v>
@@ -17568,9 +17678,9 @@
         <v>21.09090909090909</v>
       </c>
     </row>
-    <row r="75" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
-        <v>42969</v>
+        <v>42604</v>
       </c>
       <c r="B75" s="2">
         <v>5</v>
@@ -17696,9 +17806,9 @@
         <v>48.472727272727269</v>
       </c>
     </row>
-    <row r="76" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
-        <v>42970</v>
+        <v>42605</v>
       </c>
       <c r="B76" s="2">
         <v>4</v>
@@ -17824,9 +17934,9 @@
         <v>133.56363636363636</v>
       </c>
     </row>
-    <row r="77" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
-        <v>42971</v>
+        <v>42606</v>
       </c>
       <c r="B77" s="2">
         <v>7</v>
@@ -17952,9 +18062,9 @@
         <v>172.83636363636364</v>
       </c>
     </row>
-    <row r="78" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
-        <v>42972</v>
+        <v>42607</v>
       </c>
       <c r="B78" s="2">
         <v>3</v>
@@ -18080,9 +18190,9 @@
         <v>199.01818181818183</v>
       </c>
     </row>
-    <row r="79" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
-        <v>42973</v>
+        <v>42608</v>
       </c>
       <c r="B79" s="2">
         <v>4</v>
@@ -18208,9 +18318,9 @@
         <v>199.01818181818183</v>
       </c>
     </row>
-    <row r="80" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
-        <v>42974</v>
+        <v>42609</v>
       </c>
       <c r="B80" s="2">
         <v>3</v>
@@ -18336,9 +18446,9 @@
         <v>303.9878787878788</v>
       </c>
     </row>
-    <row r="81" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
-        <v>42975</v>
+        <v>42610</v>
       </c>
       <c r="B81" s="2">
         <v>4</v>
@@ -18464,9 +18574,9 @@
         <v>431.01060606060605</v>
       </c>
     </row>
-    <row r="82" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
-        <v>42976</v>
+        <v>42611</v>
       </c>
       <c r="B82" s="2">
         <v>6</v>
@@ -18592,9 +18702,9 @@
         <v>640.87424242424242</v>
       </c>
     </row>
-    <row r="83" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
-        <v>42977</v>
+        <v>42612</v>
       </c>
       <c r="B83" s="2">
         <v>5</v>
@@ -18720,9 +18830,9 @@
         <v>1027.6378787878789</v>
       </c>
     </row>
-    <row r="84" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
-        <v>42978</v>
+        <v>42613</v>
       </c>
       <c r="B84" s="2">
         <v>4</v>
@@ -18848,9 +18958,9 @@
         <v>1231.6378787878789</v>
       </c>
     </row>
-    <row r="85" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
-        <v>42979</v>
+        <v>42614</v>
       </c>
       <c r="B85" s="2">
         <v>4</v>
@@ -18976,9 +19086,9 @@
         <v>1576.5469696969699</v>
       </c>
     </row>
-    <row r="86" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
-        <v>42980</v>
+        <v>42615</v>
       </c>
       <c r="B86" s="2">
         <v>4</v>
@@ -19104,9 +19214,9 @@
         <v>1994.3651515151519</v>
       </c>
     </row>
-    <row r="87" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
-        <v>42981</v>
+        <v>42616</v>
       </c>
       <c r="B87" s="2">
         <v>2</v>
@@ -19232,9 +19342,9 @@
         <v>2611.4560606060609</v>
       </c>
     </row>
-    <row r="88" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
-        <v>42982</v>
+        <v>42617</v>
       </c>
       <c r="B88" s="2">
         <v>1</v>
@@ -19360,9 +19470,9 @@
         <v>3962.0015151515154</v>
       </c>
     </row>
-    <row r="89" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
-        <v>42983</v>
+        <v>42618</v>
       </c>
       <c r="B89" s="2">
         <v>5</v>
@@ -19488,9 +19598,9 @@
         <v>5085.0924242424244</v>
       </c>
     </row>
-    <row r="90" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
-        <v>42984</v>
+        <v>42619</v>
       </c>
       <c r="B90" s="2">
         <v>5</v>
@@ -19619,9 +19729,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="91" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
-        <v>42985</v>
+        <v>42620</v>
       </c>
       <c r="B91" s="2">
         <v>5</v>
@@ -19750,9 +19860,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="92" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
-        <v>42986</v>
+        <v>42621</v>
       </c>
       <c r="B92" s="2">
         <v>4</v>
@@ -19881,9 +19991,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="93" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
-        <v>42987</v>
+        <v>42622</v>
       </c>
       <c r="B93" s="2">
         <v>4</v>
@@ -20009,9 +20119,9 @@
         <v>9194.5365800865784</v>
       </c>
     </row>
-    <row r="94" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
-        <v>42988</v>
+        <v>42623</v>
       </c>
       <c r="B94" s="2">
         <v>4</v>
@@ -20137,9 +20247,9 @@
         <v>10460.26385281385</v>
       </c>
     </row>
-    <row r="95" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
-        <v>42989</v>
+        <v>42624</v>
       </c>
       <c r="B95" s="2">
         <v>4</v>
@@ -20265,9 +20375,9 @@
         <v>12537.718398268396</v>
       </c>
     </row>
-    <row r="96" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
-        <v>42990</v>
+        <v>42625</v>
       </c>
       <c r="B96" s="2">
         <v>4</v>
@@ -20396,9 +20506,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="97" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
-        <v>42991</v>
+        <v>42626</v>
       </c>
       <c r="B97" s="2">
         <v>3</v>
@@ -20524,9 +20634,9 @@
         <v>13317.172943722942</v>
       </c>
     </row>
-    <row r="98" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
-        <v>42992</v>
+        <v>42627</v>
       </c>
       <c r="B98" s="2">
         <v>2</v>
@@ -20655,9 +20765,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="99" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
-        <v>42993</v>
+        <v>42628</v>
       </c>
       <c r="B99" s="2">
         <v>4</v>
@@ -20783,9 +20893,9 @@
         <v>14113.150216450214</v>
       </c>
     </row>
-    <row r="100" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
-        <v>42994</v>
+        <v>42629</v>
       </c>
       <c r="B100" s="2">
         <v>2</v>
@@ -20911,9 +21021,9 @@
         <v>14597.877489177486</v>
       </c>
     </row>
-    <row r="101" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
-        <v>42995</v>
+        <v>42630</v>
       </c>
       <c r="B101" s="2">
         <v>1</v>
@@ -21039,9 +21149,9 @@
         <v>14772.422943722941</v>
       </c>
     </row>
-    <row r="102" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
-        <v>42996</v>
+        <v>42631</v>
       </c>
       <c r="B102" s="2">
         <v>3</v>
@@ -21167,9 +21277,9 @@
         <v>15229.489610389608</v>
       </c>
     </row>
-    <row r="103" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
-        <v>42997</v>
+        <v>42632</v>
       </c>
       <c r="B103" s="2">
         <v>2</v>
@@ -21295,9 +21405,9 @@
         <v>16391.035064935062</v>
       </c>
     </row>
-    <row r="104" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
-        <v>42998</v>
+        <v>42633</v>
       </c>
       <c r="B104" s="2">
         <v>0</v>
@@ -21423,9 +21533,9 @@
         <v>16580.853246753242</v>
       </c>
     </row>
-    <row r="105" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
-        <v>42999</v>
+        <v>42634</v>
       </c>
       <c r="B105" s="2">
         <v>1</v>
@@ -21551,9 +21661,9 @@
         <v>16925.580519480514</v>
       </c>
     </row>
-    <row r="106" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
-        <v>43000</v>
+        <v>42635</v>
       </c>
       <c r="B106" s="2">
         <v>5</v>
@@ -21679,9 +21789,9 @@
         <v>17468.562337662333</v>
       </c>
     </row>
-    <row r="107" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
-        <v>43001</v>
+        <v>42636</v>
       </c>
       <c r="B107" s="2">
         <v>2</v>
@@ -21807,9 +21917,9 @@
         <v>17901.471428571425</v>
       </c>
     </row>
-    <row r="108" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
-        <v>43002</v>
+        <v>42637</v>
       </c>
       <c r="B108" s="2">
         <v>1</v>
@@ -21935,9 +22045,9 @@
         <v>18326.925974025969</v>
       </c>
     </row>
-    <row r="109" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
-        <v>43003</v>
+        <v>42638</v>
       </c>
       <c r="B109" s="2">
         <v>4</v>
@@ -22063,9 +22173,9 @@
         <v>18764.107792207789</v>
       </c>
     </row>
-    <row r="110" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
-        <v>43004</v>
+        <v>42639</v>
       </c>
       <c r="B110" s="2">
         <v>4</v>
@@ -22191,9 +22301,9 @@
         <v>18918.80779220779</v>
       </c>
     </row>
-    <row r="111" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
-        <v>43005</v>
+        <v>42640</v>
       </c>
       <c r="B111" s="2">
         <v>5</v>
@@ -22319,9 +22429,9 @@
         <v>19104.371428571427</v>
       </c>
     </row>
-    <row r="112" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
-        <v>43006</v>
+        <v>42641</v>
       </c>
       <c r="B112" s="2">
         <v>6</v>
@@ -22447,9 +22557,9 @@
         <v>19313.371428571427</v>
       </c>
     </row>
-    <row r="113" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
-        <v>43007</v>
+        <v>42642</v>
       </c>
       <c r="B113" s="2">
         <v>3</v>
@@ -22575,9 +22685,9 @@
         <v>19570.462337662335</v>
       </c>
     </row>
-    <row r="114" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
-        <v>43008</v>
+        <v>42643</v>
       </c>
       <c r="B114" s="2">
         <v>7</v>
@@ -22703,9 +22813,9 @@
         <v>19876.48831168831</v>
       </c>
     </row>
-    <row r="115" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
-        <v>43009</v>
+        <v>42644</v>
       </c>
       <c r="B115" s="2">
         <v>2</v>
@@ -22831,9 +22941,9 @@
         <v>19948.48831168831</v>
       </c>
     </row>
-    <row r="116" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
-        <v>43010</v>
+        <v>42645</v>
       </c>
       <c r="B116" s="2">
         <v>3</v>
@@ -22969,39 +23079,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="912" topLeftCell="A81" activePane="bottomLeft"/>
+      <pane ySplit="915" activePane="bottomLeft"/>
       <selection activeCell="X6" sqref="X6"/>
-      <selection pane="bottomLeft" activeCell="AJ117" sqref="AJ117"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="2"/>
-    <col min="8" max="8" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="2"/>
+    <col min="8" max="8" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" style="2"/>
-    <col min="14" max="14" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="2"/>
+    <col min="14" max="14" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.88671875" style="2"/>
+    <col min="17" max="17" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
@@ -23012,7 +23122,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
@@ -23062,7 +23172,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="48">
         <v>42898</v>
       </c>
@@ -23104,7 +23214,7 @@
         <v>8.2987041727114012E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="48">
         <v>42899</v>
       </c>
@@ -23146,7 +23256,7 @@
         <v>1.5183555041923823E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="48">
         <v>42900</v>
       </c>
@@ -23188,7 +23298,7 @@
         <v>2.0654552607637267E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="48">
         <v>42901</v>
       </c>
@@ -23230,7 +23340,7 @@
         <v>3.0133516929356511E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="48">
         <v>42902</v>
       </c>
@@ -23272,7 +23382,7 @@
         <v>4.2661486636012685E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="48">
         <v>42903</v>
       </c>
@@ -23314,7 +23424,7 @@
         <v>5.3910841181243702E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="48">
         <v>42904</v>
       </c>
@@ -23356,7 +23466,7 @@
         <v>6.6426516511347705E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="48">
         <v>42905</v>
       </c>
@@ -23398,7 +23508,7 @@
         <v>8.2212496004327618E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="48">
         <v>42906</v>
       </c>
@@ -23440,7 +23550,7 @@
         <v>0.1025842779512651</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="48">
         <v>42907</v>
       </c>
@@ -23482,7 +23592,7 @@
         <v>0.1206938946126042</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="48">
         <v>42908</v>
       </c>
@@ -23524,7 +23634,7 @@
         <v>0.14900784381224028</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="48">
         <v>42909</v>
       </c>
@@ -23566,7 +23676,7 @@
         <v>0.18085027908234774</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="48">
         <v>42910</v>
       </c>
@@ -23608,7 +23718,7 @@
         <v>0.20386535198800068</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="48">
         <v>42911</v>
       </c>
@@ -23650,7 +23760,7 @@
         <v>0.23188423615038481</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="48">
         <v>42912</v>
       </c>
@@ -23692,7 +23802,7 @@
         <v>0.25467801027809878</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="48">
         <v>42913</v>
       </c>
@@ -23734,7 +23844,7 @@
         <v>0.28218053062529197</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="48">
         <v>42914</v>
       </c>
@@ -23776,7 +23886,7 @@
         <v>0.31253534633258745</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="48">
         <v>42915</v>
       </c>
@@ -23818,7 +23928,7 @@
         <v>0.34410730531854727</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="48">
         <v>42916</v>
       </c>
@@ -23860,7 +23970,7 @@
         <v>0.37716688386731911</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="48">
         <v>42917</v>
       </c>
@@ -23902,7 +24012,7 @@
         <v>0.40410386289311268</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="48">
         <v>42918</v>
       </c>
@@ -23944,7 +24054,7 @@
         <v>0.43156950011064937</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="48">
         <v>42919</v>
       </c>
@@ -23986,7 +24096,7 @@
         <v>0.4588261329267993</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="48">
         <v>42920</v>
       </c>
@@ -24028,7 +24138,7 @@
         <v>0.49934839804273523</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="48">
         <v>42921</v>
       </c>
@@ -24070,7 +24180,7 @@
         <v>0.5290147286631095</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="48">
         <v>42922</v>
       </c>
@@ -24112,7 +24222,7 @@
         <v>0.56806166859278562</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="48">
         <v>42923</v>
       </c>
@@ -24154,7 +24264,7 @@
         <v>0.60446531756374633</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="48">
         <v>42924</v>
       </c>
@@ -24196,7 +24306,7 @@
         <v>0.62563623398657453</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="48">
         <v>42925</v>
       </c>
@@ -24238,7 +24348,7 @@
         <v>0.65478620079175787</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="48">
         <v>42926</v>
       </c>
@@ -24280,7 +24390,7 @@
         <v>0.67935036514298364</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="48">
         <v>42927</v>
       </c>
@@ -24322,7 +24432,7 @@
         <v>0.70650864294671623</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="48">
         <v>42928</v>
       </c>
@@ -24364,7 +24474,7 @@
         <v>0.73472423713393498</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="48">
         <v>42929</v>
       </c>
@@ -24406,7 +24516,7 @@
         <v>0.75980476530035157</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="48">
         <v>42930</v>
       </c>
@@ -24448,7 +24558,7 @@
         <v>0.78675403870269733</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="48">
         <v>42931</v>
       </c>
@@ -24490,7 +24600,7 @@
         <v>0.80837984705795574</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="48">
         <v>42932</v>
       </c>
@@ -24532,7 +24642,7 @@
         <v>0.82566574049029973</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="48">
         <v>42933</v>
       </c>
@@ -24574,7 +24684,7 @@
         <v>0.84227544321227465</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="48">
         <v>42934</v>
       </c>
@@ -24616,7 +24726,7 @@
         <v>0.85661068627209913</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="48">
         <v>42935</v>
       </c>
@@ -24658,7 +24768,7 @@
         <v>0.86869605842287734</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="48">
         <v>42936</v>
       </c>
@@ -24700,7 +24810,7 @@
         <v>0.87912168973911331</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="48">
         <v>42937</v>
       </c>
@@ -24742,7 +24852,7 @@
         <v>0.8897809142098404</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="48">
         <v>42938</v>
       </c>
@@ -24784,7 +24894,7 @@
         <v>0.89986230298261571</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="48">
         <v>42939</v>
       </c>
@@ -24826,7 +24936,7 @@
         <v>0.90789053087117955</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="48">
         <v>42940</v>
       </c>
@@ -24868,7 +24978,7 @@
         <v>0.91810715778602869</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="48">
         <v>42941</v>
       </c>
@@ -24910,7 +25020,7 @@
         <v>0.92650421697115737</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="48">
         <v>42942</v>
       </c>
@@ -24952,7 +25062,7 @@
         <v>0.93520863557009026</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="48">
         <v>42943</v>
       </c>
@@ -24994,7 +25104,7 @@
         <v>0.94343357348348866</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="48">
         <v>42944</v>
       </c>
@@ -25036,7 +25146,7 @@
         <v>0.94996188743268828</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="48">
         <v>42945</v>
       </c>
@@ -25078,7 +25188,7 @@
         <v>0.95464604489906313</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="48">
         <v>42946</v>
       </c>
@@ -25120,7 +25230,7 @@
         <v>0.95999409869925501</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="48">
         <v>42947</v>
       </c>
@@ -25162,7 +25272,7 @@
         <v>0.96365782291180013</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="48">
         <v>42948</v>
       </c>
@@ -25204,7 +25314,7 @@
         <v>0.96687894956846743</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="48">
         <v>42949</v>
       </c>
@@ -25246,7 +25356,7 @@
         <v>0.96973124492856966</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="48">
         <v>42950</v>
       </c>
@@ -25288,7 +25398,7 @@
         <v>0.97265730654798499</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="48">
         <v>42951</v>
       </c>
@@ -25330,7 +25440,7 @@
         <v>0.97650544640881265</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="48">
         <v>42952</v>
       </c>
@@ -25372,7 +25482,7 @@
         <v>0.97976345619513638</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="48">
         <v>42953</v>
       </c>
@@ -25414,7 +25524,7 @@
         <v>0.98260345717868647</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="48">
         <v>42954</v>
       </c>
@@ -25456,7 +25566,7 @@
         <v>0.98533280877326712</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="48">
         <v>42955</v>
       </c>
@@ -25498,7 +25608,7 @@
         <v>0.98683272271263123</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="48">
         <v>42956</v>
       </c>
@@ -25540,7 +25650,7 @@
         <v>0.98829575352233889</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="48">
         <v>42957</v>
       </c>
@@ -25582,7 +25692,7 @@
         <v>0.99012761562861151</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="48">
         <v>42958</v>
       </c>
@@ -25624,7 +25734,7 @@
         <v>0.99138164203693235</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="48">
         <v>42959</v>
       </c>
@@ -25666,7 +25776,7 @@
         <v>0.99263566844525319</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="48">
         <v>42960</v>
       </c>
@@ -25708,7 +25818,7 @@
         <v>0.9940864048784086</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="48">
         <v>42961</v>
       </c>
@@ -25750,7 +25860,7 @@
         <v>0.99535272566328159</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="48">
         <v>42962</v>
       </c>
@@ -25792,7 +25902,7 @@
         <v>0.99604121075020291</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="48">
         <v>42963</v>
       </c>
@@ -25834,7 +25944,7 @@
         <v>0.99671740146057197</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="48">
         <v>42964</v>
       </c>
@@ -25876,7 +25986,7 @@
         <v>0.99709852713368907</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="48">
         <v>42965</v>
       </c>
@@ -25918,7 +26028,7 @@
         <v>0.99743047530059747</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="48">
         <v>42966</v>
       </c>
@@ -25960,7 +26070,7 @@
         <v>0.99792225036268412</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="48">
         <v>42967</v>
       </c>
@@ -26002,7 +26112,7 @@
         <v>0.99827878728269692</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="48">
         <v>42968</v>
       </c>
@@ -26044,7 +26154,7 @@
         <v>0.99868450170891832</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="48">
         <v>42969</v>
       </c>
@@ -26086,7 +26196,7 @@
         <v>0.99889350611030514</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="48">
         <v>42970</v>
       </c>
@@ -26128,7 +26238,7 @@
         <v>0.99911480488824411</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="48">
         <v>42971</v>
       </c>
@@ -26170,7 +26280,7 @@
         <v>0.9992131599006614</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="48">
         <v>42972</v>
       </c>
@@ -26212,7 +26322,7 @@
         <v>0.99927463178342224</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="48">
         <v>42973</v>
       </c>
@@ -26254,7 +26364,7 @@
         <v>0.99942216430204822</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="48">
         <v>42974</v>
       </c>
@@ -26296,7 +26406,7 @@
         <v>0.99959428557377861</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="48">
         <v>42975</v>
       </c>
@@ -26338,7 +26448,7 @@
         <v>0.99969264058619589</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="48">
         <v>42976</v>
       </c>
@@ -26380,7 +26490,7 @@
         <v>0.99972952371585233</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="48">
         <v>42977</v>
       </c>
@@ -26422,7 +26532,7 @@
         <v>0.99979099559861317</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="48">
         <v>42978</v>
       </c>
@@ -26464,7 +26574,7 @@
         <v>0.99985246748137402</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="48">
         <v>42979</v>
       </c>
@@ -26524,7 +26634,7 @@
         <v>1.4730771641697487E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="48">
         <v>42980</v>
       </c>
@@ -26584,7 +26694,7 @@
         <v>3.3285275496771766E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="48">
         <v>42981</v>
       </c>
@@ -26644,7 +26754,7 @@
         <v>5.5976932238450447E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" s="48">
         <v>42982</v>
       </c>
@@ -26704,7 +26814,7 @@
         <v>8.1677427443114153E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" s="48">
         <v>42983</v>
       </c>
@@ -26764,7 +26874,7 @@
         <v>0.11126433899580017</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="48">
         <v>42984</v>
       </c>
@@ -26824,7 +26934,7 @@
         <v>0.1441735096846988</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="48">
         <v>42985</v>
       </c>
@@ -26884,7 +26994,7 @@
         <v>0.17156647652479157</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="48">
         <v>42986</v>
       </c>
@@ -26944,7 +27054,7 @@
         <v>0.20497712029085438</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="48">
         <v>42987</v>
       </c>
@@ -27004,7 +27114,7 @@
         <v>0.2363818717482605</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="48">
         <v>42988</v>
       </c>
@@ -27064,7 +27174,7 @@
         <v>0.27286403811195387</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="48">
         <v>42989</v>
       </c>
@@ -27124,7 +27234,7 @@
         <v>0.33109759919764309</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" s="48">
         <v>42990</v>
       </c>
@@ -27184,7 +27294,7 @@
         <v>0.36971102613928414</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" s="48">
         <v>42991</v>
       </c>
@@ -27244,7 +27354,7 @@
         <v>0.40443803673290291</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" s="48">
         <v>42992</v>
       </c>
@@ -27304,7 +27414,7 @@
         <v>0.43621889299818217</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" s="48">
         <v>42993</v>
       </c>
@@ -27364,7 +27474,7 @@
         <v>0.47746505359493513</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" s="48">
         <v>42994</v>
       </c>
@@ -27424,7 +27534,7 @@
         <v>0.52698551996489684</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" s="48">
         <v>42995</v>
       </c>
@@ -27484,7 +27594,7 @@
         <v>0.56290352911678054</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" s="48">
         <v>42996</v>
       </c>
@@ -27544,7 +27654,7 @@
         <v>0.60233184980881338</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" s="48">
         <v>42997</v>
       </c>
@@ -27604,7 +27714,7 @@
         <v>0.64558390271422306</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" s="48">
         <v>42998</v>
       </c>
@@ -27664,7 +27774,7 @@
         <v>0.67698865417162912</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" s="48">
         <v>42999</v>
       </c>
@@ -27724,7 +27834,7 @@
         <v>0.70745314360935252</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" s="48">
         <v>43000</v>
       </c>
@@ -27784,7 +27894,7 @@
         <v>0.74186673352974364</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" s="48">
         <v>43001</v>
       </c>
@@ -27844,7 +27954,7 @@
         <v>0.7742117470068326</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" s="48">
         <v>43002</v>
       </c>
@@ -27904,7 +28014,7 @@
         <v>0.8154579076035855</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" s="48">
         <v>43003</v>
       </c>
@@ -27964,7 +28074,7 @@
         <v>0.84416724127123421</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" s="48">
         <v>43004</v>
       </c>
@@ -28024,7 +28134,7 @@
         <v>0.87112141916880836</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110" s="48">
         <v>43005</v>
       </c>
@@ -28084,7 +28194,7 @@
         <v>0.90171127687582275</v>
       </c>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111" s="48">
         <v>43006</v>
       </c>
@@ -28144,7 +28254,7 @@
         <v>0.91988967592302384</v>
       </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112" s="48">
         <v>43007</v>
       </c>
@@ -28204,7 +28314,7 @@
         <v>0.94684385382059799</v>
       </c>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A113" s="48">
         <v>43008</v>
       </c>
@@ -28264,7 +28374,7 @@
         <v>0.96815645960007524</v>
       </c>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A114" s="48">
         <v>43009</v>
       </c>
@@ -28324,7 +28434,7 @@
         <v>0.9883407509559331</v>
       </c>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A115" s="48">
         <v>43010</v>
       </c>
@@ -28384,10 +28494,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A116" s="49"/>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A117" s="49"/>
     </row>
   </sheetData>

</xml_diff>